<commit_message>
foxed page num bugs
</commit_message>
<xml_diff>
--- a/excel/pageList.xlsx
+++ b/excel/pageList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="127">
   <si>
     <t>title</t>
   </si>
@@ -292,6 +292,161 @@
   </si>
   <si>
     <t>這是第四篇文章18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>img/index/test4.jpg</t>
+  </si>
+  <si>
+    <t>2014/2/28</t>
+  </si>
+  <si>
+    <t>2014/2/29</t>
+  </si>
+  <si>
+    <t>2014/2/30</t>
+  </si>
+  <si>
+    <t>2014/2/31</t>
+  </si>
+  <si>
+    <t>2014/2/32</t>
+  </si>
+  <si>
+    <t>2014/2/33</t>
+  </si>
+  <si>
+    <t>2014/2/34</t>
+  </si>
+  <si>
+    <t>2014/2/35</t>
+  </si>
+  <si>
+    <t>2014/2/36</t>
+  </si>
+  <si>
+    <t>2014/2/37</t>
+  </si>
+  <si>
+    <t>這是第五篇文章21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第六篇文章22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第五篇文章23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第六篇文章24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第五篇文章25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第六篇文章26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第五篇文章27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第六篇文章28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag-ill</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第篇文章28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這是第篇文章29</t>
+  </si>
+  <si>
+    <t>這是第篇文章30</t>
+  </si>
+  <si>
+    <t>這是第篇文章31</t>
+  </si>
+  <si>
+    <t>這是第篇文章32</t>
+  </si>
+  <si>
+    <t>這是第篇文章33</t>
+  </si>
+  <si>
+    <t>這是第篇文章34</t>
+  </si>
+  <si>
+    <t>這是第篇文章35</t>
+  </si>
+  <si>
+    <t>這是第篇文章36</t>
+  </si>
+  <si>
+    <t>這是第篇文章37</t>
+  </si>
+  <si>
+    <t>這是第篇文章38</t>
+  </si>
+  <si>
+    <t>這是第篇文章39</t>
+  </si>
+  <si>
+    <t>2014/2/38</t>
+  </si>
+  <si>
+    <t>這是第篇文章40</t>
+  </si>
+  <si>
+    <t>2014/2/39</t>
+  </si>
+  <si>
+    <t>這是第篇文章41</t>
+  </si>
+  <si>
+    <t>2014/2/40</t>
+  </si>
+  <si>
+    <t>這是第篇文章42</t>
+  </si>
+  <si>
+    <t>2014/2/41</t>
+  </si>
+  <si>
+    <t>這是第篇文章43</t>
+  </si>
+  <si>
+    <t>2014/2/42</t>
+  </si>
+  <si>
+    <t>這是第篇文章44</t>
+  </si>
+  <si>
+    <t>2014/2/43</t>
+  </si>
+  <si>
+    <t>這是第篇文章45</t>
+  </si>
+  <si>
+    <t>2014/2/44</t>
+  </si>
+  <si>
+    <t>這是第篇文章46</t>
+  </si>
+  <si>
+    <t>2014/2/45</t>
+  </si>
+  <si>
+    <t>tag-others</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -679,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1116,6 +1271,546 @@
         <v>44</v>
       </c>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add article:sublimetext package, and add prettify code style
</commit_message>
<xml_diff>
--- a/excel/pageList.xlsx
+++ b/excel/pageList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>title</t>
   </si>
@@ -61,6 +61,26 @@
   </si>
   <si>
     <t>/img/articles/201405/20140518_2_01.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag-web</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SublimeText Package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/articles/201405/sublimetext-package.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/img/articles/201405/20140520_1_01.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAY 20TH, 2014</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -433,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -468,19 +488,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -488,15 +508,32 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add svg-04-path-1.html, add GA check
</commit_message>
<xml_diff>
--- a/excel/pageList.xlsx
+++ b/excel/pageList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="103">
   <si>
     <t>title</t>
   </si>
@@ -405,6 +405,22 @@
   </si>
   <si>
     <t>SVG 研究之路 (4) - Path 基礎篇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVG 研究之路 (5) - Path 進階篇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/img/articles/201406/20140612_1_01.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JUN 12TH, 2014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/articles/201406/svg-05-path-2.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -777,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -815,50 +831,50 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -866,13 +882,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>85</v>
@@ -883,47 +899,47 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>76</v>
@@ -931,50 +947,50 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>64</v>
@@ -985,30 +1001,30 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>57</v>
@@ -1016,118 +1032,118 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>22</v>
@@ -1135,16 +1151,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>22</v>
@@ -1152,36 +1168,36 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1189,15 +1205,32 @@
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add css-blur.html and css-webkit-filter.html
</commit_message>
<xml_diff>
--- a/excel/pageList.xlsx
+++ b/excel/pageList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="184">
   <si>
     <t>title</t>
   </si>
@@ -718,6 +718,34 @@
   </si>
   <si>
     <t>電子時鐘效果 ( CSS 偽元素的應用 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/articles/201407/css-blur.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/img/articles/201407/20140726_1_01.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JUL 26, 2014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS 模糊效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/img/articles/201407/20140726_2_01.jpg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/articles/201407/css-webkit-filter.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSS webkit filter</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1090,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1128,67 +1156,67 @@
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,101 +1224,101 @@
         <v>155</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>155</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>116</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,16 +1326,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1315,33 +1343,33 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,33 +1377,33 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>11</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1383,16 +1411,16 @@
         <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1400,16 +1428,16 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1417,16 +1445,16 @@
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,16 +1462,16 @@
         <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1451,33 +1479,33 @@
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1485,33 +1513,33 @@
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1519,203 +1547,203 @@
         <v>11</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,50 +1751,50 @@
         <v>26</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1774,13 +1802,13 @@
         <v>15</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>139</v>
@@ -1788,52 +1816,86 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>